<commit_message>
Updated voice script file
</commit_message>
<xml_diff>
--- a/Voice/voice script.xlsx
+++ b/Voice/voice script.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEO JOFEH\Documents\PACTICS\bc system demo\Voice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A84CF1B-7A76-48C5-92B3-1532AB39B86F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A76680-FE57-4FB4-AE64-91A3E724E471}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1035" yWindow="1035" windowWidth="13230" windowHeight="14025" xr2:uid="{E4F7D997-665B-4B5E-A4CC-9B38ECB6B4B8}"/>
   </bookViews>
@@ -199,6 +199,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>20610</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41722AF2-9F6C-4F90-BF11-A649513640A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10144125" y="0"/>
+          <a:ext cx="6288060" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -501,14 +556,14 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
     <col min="5" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="2" customWidth="1"/>
@@ -828,5 +883,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implement interaction timer with file and dweet reporting
</commit_message>
<xml_diff>
--- a/Voice/voice script.xlsx
+++ b/Voice/voice script.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEO JOFEH\Documents\PACTICS\bc system demo\Voice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AEA2A5-9868-434C-A897-CE74FD3F95E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7C76F-DEF2-42D1-95BC-1D140FA3AB0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4F7D997-665B-4B5E-A4CC-9B38ECB6B4B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Use case</t>
   </si>
@@ -78,15 +78,6 @@
     <t>Integers for counting</t>
   </si>
   <si>
-    <t>General use</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Everything</t>
-  </si>
-  <si>
     <t>When they user has tried to commit an operation but they are missing information.</t>
   </si>
   <si>
@@ -178,13 +169,26 @@
   </si>
   <si>
     <t>voice test 1</t>
+  </si>
+  <si>
+    <t>Voice/finishedthankyou_KH.mp3</t>
+  </si>
+  <si>
+    <t>* assumes script is called locally - this ought to be fixed soon.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,16 +210,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -223,21 +241,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -256,16 +294,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>90488</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>20610</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>282548</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -294,8 +332,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10144125" y="0"/>
-          <a:ext cx="6288060" cy="10058400"/>
+          <a:off x="14127957" y="23812"/>
+          <a:ext cx="6264247" cy="10058400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -604,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAAB67C-38A6-45CB-8DB2-2B4578A53B84}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,14 +653,16 @@
     <col min="1" max="1" width="43" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="24.140625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,13 +682,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -656,19 +696,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -676,70 +716,76 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -747,105 +793,105 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="G11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="G12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -971,7 +1017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>60</v>
       </c>
@@ -979,7 +1025,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>70</v>
       </c>
@@ -987,7 +1033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>80</v>
       </c>
@@ -995,7 +1041,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>90</v>
       </c>
@@ -1003,7 +1049,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>100</v>
       </c>
@@ -1011,21 +1057,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
add support for announcing numbers in english and khmer
But haven't yet added all the sound files for khmer language.
</commit_message>
<xml_diff>
--- a/Voice/voice script.xlsx
+++ b/Voice/voice script.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEO JOFEH\Documents\PACTICS\bc system demo\Voice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7C76F-DEF2-42D1-95BC-1D140FA3AB0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E005A232-BC19-4F38-B05A-24A041DE9955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4F7D997-665B-4B5E-A4CC-9B38ECB6B4B8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Use case</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>* assumes script is called locally - this ought to be fixed soon.</t>
+  </si>
+  <si>
+    <t>to confirm a good input</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>still to add, suggested by bong Thavy</t>
   </si>
 </sst>
 </file>
@@ -302,7 +311,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>282548</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -644,15 +653,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAAB67C-38A6-45CB-8DB2-2B4578A53B84}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -751,7 +760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
@@ -768,7 +777,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -892,6 +901,20 @@
       </c>
       <c r="H14" s="2" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>